<commit_message>
tuoi tre 18/9/2022 update
</commit_message>
<xml_diff>
--- a/TT_189/TT_189.xlsx
+++ b/TT_189/TT_189.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam tu\KLTN\data\TT_189\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C65DEB0-8B1D-4B92-AA66-939CA6F8C02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BEE64C-CBA9-4463-ADDF-BB6C688B8478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29890" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1836" uniqueCount="786">
   <si>
     <t>id</t>
   </si>
@@ -2197,6 +2197,192 @@
   </si>
   <si>
     <t>https://cdn.tuoitre.vn/2022/9/9/queen-4-166266236721929178125.jpg</t>
+  </si>
+  <si>
+    <t>00032dk3wa-16567386366061815777354.jpg</t>
+  </si>
+  <si>
+    <t>cuộc họp báo ở điện Kremlin</t>
+  </si>
+  <si>
+    <t>30/6/2022</t>
+  </si>
+  <si>
+    <t>Tổng thống Indonesia Joko Widodo (trái) bắt tay Tổng thống Nga Vladimir Putin tại Matxcơva ngày 30-6</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/2/00032dk3wa-16567386366061815777354.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/nga-chuyen-dong-tien-dau-tu-vao-indonesia-20220702121306658.htm</t>
+  </si>
+  <si>
+    <t>joko-widodo-putin-1656606035951875071377.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/6/30/joko-widodo-putin-1656606035951875071377.jpg</t>
+  </si>
+  <si>
+    <t>Tổng thống Widodo (trái) trong cuộc gặp với Tổng thống Putin ngày 30-6</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tong-thong-indonesia-mang-thong-diep-cua-ong-zelensky-chuyen-cho-ong-putin-2022063023192303.htm</t>
+  </si>
+  <si>
+    <t>indonesia-16566385074701815286573.jpg</t>
+  </si>
+  <si>
+    <t>Tổng thống Nga Vladimir Putin (phải) bắt tay Tổng thống Indonesia Joko Widodo sau cuộc họp báo tại Điện Kremlin ở Matxcơva, Nga ngày 30-6</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/1/indonesia-16566385074701815286573.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tong-thong-indonesia-ong-putin-dong-y-mo-tuyen-duong-bien-xuat-khau-lua-mi-ukraine-20220701081136298.htm</t>
+  </si>
+  <si>
+    <t>putin-shoigu-16569381547931248053283.jpg</t>
+  </si>
+  <si>
+    <t>cuộc gặp với Bộ trưởng Quốc phòng Shoigu</t>
+  </si>
+  <si>
+    <t>4/7/2022</t>
+  </si>
+  <si>
+    <t>Tổng thống Putin trong cuộc gặp với Bộ trưởng Quốc phòng Shoigu ngày 4-7</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/4/putin-shoigu-16569381547931248053283.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tong-thong-putin-ra-lenh-tiep-tuc-tan-cong-sau-khi-kiem-soat-toan-bo-lugansk-20220704193821861.htm</t>
+  </si>
+  <si>
+    <t>00032dg3we-16565661801761614480921.jpg</t>
+  </si>
+  <si>
+    <t>cuộc họp báo ở Ashgabat</t>
+  </si>
+  <si>
+    <t>Ashgabat</t>
+  </si>
+  <si>
+    <t>29/6/2022</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Tổng thống Nga Vladimir Putin có mặt tại Turkmenistan ngày 29-6</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/6/30/00032dg3we-16565661801761614480921.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/tong-thong-putin-khong-co-han-chot-cho-chien-su-o-ukraine-20220630122101847.htm</t>
+  </si>
+  <si>
+    <t>62bcf2712030274eca71750a-16565661801642015394032.jpg</t>
+  </si>
+  <si>
+    <t>Ông Putin khẳng định chiến dịch quân sự của Nga vẫn đang đi theo kế hoạch</t>
+  </si>
+  <si>
+    <t>Kremlin</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/6/30/62bcf2712030274eca71750a-16565661801642015394032.jpg</t>
+  </si>
+  <si>
+    <t>00032dg68r-2read-only-1656898179742197210126.jpg</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Tây Ban Nha</t>
+  </si>
+  <si>
+    <t>Thượng đỉnh Mỹ - Hàn - Nhật bên lề Thượng đỉnh G7 ở Madrid ngày 29-6</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/4/00032dg68r-2read-only-1656898179742197210126.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/kho-co-nato-chau-a-nhu-trieu-tien-lo-20220704083402488.htm</t>
+  </si>
+  <si>
+    <t>2022-07-01t033941z1545829232rc2r2v97m93srtrmadp3hongkong-anniversary-1-16566707016651866380820.jpg</t>
+  </si>
+  <si>
+    <t>buổi lễ nhậm chức của Trưởng đặc khu hành chính Hong Kong Lý Gia Siêu</t>
+  </si>
+  <si>
+    <t>1/7/2022</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Chủ tịch Trung Quốc Tập Cận Bình sau bài phát biểu tại buổi lễ nhậm chức của Trưởng đặc khu hành chính Hong Kong Lý Gia Siêu ngày 1-7</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/1/2022-07-01t033941z1545829232rc2r2v97m93srtrmadp3hongkong-anniversary-1-16566707016651866380820.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/chu-tich-tap-can-binh-khong-co-ly-do-de-thay-doi-mot-quoc-gia-hai-che-do-o-hong-kong-20220701172449009.htm</t>
+  </si>
+  <si>
+    <t>2022-07-01t055832z1718483302rc2q2v97nppqrtrmadp3hongkong-anniversary-2read-only-16567263716491741415162.jpg</t>
+  </si>
+  <si>
+    <t>Ông Lý Gia Siêu (trái) tuyên thệ làm trưởng đặc khu Hong Kong trước sự chứng kiến của Chủ tịch Tập Cận Bình vào ngày 1-7</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/2/2022-07-01t055832z1718483302rc2q2v97nppqrtrmadp3hongkong-anniversary-2read-only-16567263716491741415162.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ban-sac-hong-kong-25-nam-sau-20220702084902305.htm</t>
+  </si>
+  <si>
+    <t>2022-06-22t131511z1730849069rc210t9yccnirtrmadp3china-summit-brics-1657025397877780461087.jpg</t>
+  </si>
+  <si>
+    <t>Nga cho biết Chủ tịch Trung Quốc Tập Cận Bình sẽ đến thăm nước này khi các biện pháp chống dịch COVID-19 được nới lỏng</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/5/2022-06-22t131511z1730849069rc210t9yccnirtrmadp3china-summit-brics-1657025397877780461087.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/dien-kremlin-bac-thong-tin-ong-tap-tu-choi-den-nga-20220705195230509.htm</t>
+  </si>
+  <si>
+    <t>tq-tap-can-binh-feng-li-getty-16589768881071354517134.jpg</t>
+  </si>
+  <si>
+    <t>Chủ tịch Trung Quốc Tập Cận Bình</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/28/tq-tap-can-binh-feng-li-getty-16589768881071354517134.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/ong-tap-can-binh-trung-quoc-gat-hai-duoc-nhung-thang-loi-tot-nhat-the-gioi-ve-chong-covid-19-20220728095726823.htm</t>
+  </si>
+  <si>
+    <t>biden-1657006723249381254278.jpg</t>
+  </si>
+  <si>
+    <t>lễ Quốc khánh Mỹ</t>
+  </si>
+  <si>
+    <t>Tổng thống Mỹ Joe Biden và Đệ nhất phu nhân Mỹ Jill Biden xem pháo hoa từ Nhà Trắng vào ngày 4-7 nhân dịp Quốc khánh Mỹ</t>
+  </si>
+  <si>
+    <t>https://cdn.tuoitre.vn/2022/7/5/biden-1657006723249381254278.jpg</t>
+  </si>
+  <si>
+    <t>https://tuoitre.vn/thong-diep-quoc-khanh-cua-ong-biden-nguoi-my-hien-doan-ket-hon-la-chia-re-20220705143610379.htm</t>
   </si>
 </sst>
 </file>
@@ -2288,7 +2474,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2304,6 +2490,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2328,7 +2520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2358,12 +2550,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2585,8 +2782,8 @@
   </sheetPr>
   <dimension ref="A1:N999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -2683,10 +2880,10 @@
       <c r="L2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="30"/>
+      <c r="N2" s="35"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="5" t="s">
@@ -2723,10 +2920,10 @@
       <c r="L3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="29" t="s">
+      <c r="M3" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="30"/>
+      <c r="N3" s="35"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="5" t="s">
@@ -2763,10 +2960,10 @@
       <c r="L4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="30"/>
+      <c r="N4" s="35"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="5" t="s">
@@ -2803,10 +3000,10 @@
       <c r="L5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="M5" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="30"/>
+      <c r="N5" s="35"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="5" t="s">
@@ -2843,10 +3040,10 @@
       <c r="L6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="N6" s="30"/>
+      <c r="N6" s="35"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="5" t="s">
@@ -2883,10 +3080,10 @@
       <c r="L7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="30"/>
+      <c r="N7" s="35"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="5" t="s">
@@ -2923,10 +3120,10 @@
       <c r="L8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="30"/>
+      <c r="N8" s="35"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="5" t="s">
@@ -2963,10 +3160,10 @@
       <c r="L9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="M9" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="N9" s="30"/>
+      <c r="N9" s="35"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="5" t="s">
@@ -3003,10 +3200,10 @@
       <c r="L10" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="N10" s="30"/>
+      <c r="N10" s="35"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="5" t="s">
@@ -3043,10 +3240,10 @@
       <c r="L11" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="M11" s="29" t="s">
+      <c r="M11" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="N11" s="30"/>
+      <c r="N11" s="35"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="5" t="s">
@@ -3083,10 +3280,10 @@
       <c r="L12" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="N12" s="30"/>
+      <c r="N12" s="35"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="5" t="s">
@@ -3123,10 +3320,10 @@
       <c r="L13" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="N13" s="30"/>
+      <c r="N13" s="35"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="5" t="s">
@@ -3163,10 +3360,10 @@
       <c r="L14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="N14" s="30"/>
+      <c r="N14" s="35"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="5" t="s">
@@ -3203,10 +3400,10 @@
       <c r="L15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="N15" s="30"/>
+      <c r="N15" s="35"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="5" t="s">
@@ -3243,10 +3440,10 @@
       <c r="L16" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="29" t="s">
+      <c r="M16" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="N16" s="30"/>
+      <c r="N16" s="35"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="5" t="s">
@@ -3283,10 +3480,10 @@
       <c r="L17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="M17" s="29" t="s">
+      <c r="M17" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N17" s="30"/>
+      <c r="N17" s="35"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="5" t="s">
@@ -3323,10 +3520,10 @@
       <c r="L18" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="M18" s="29" t="s">
+      <c r="M18" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N18" s="30"/>
+      <c r="N18" s="35"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="5" t="s">
@@ -3363,10 +3560,10 @@
       <c r="L19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="M19" s="29" t="s">
+      <c r="M19" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N19" s="30"/>
+      <c r="N19" s="35"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="5" t="s">
@@ -3403,10 +3600,10 @@
       <c r="L20" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="M20" s="29" t="s">
+      <c r="M20" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="30"/>
+      <c r="N20" s="35"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5" t="s">
@@ -3443,10 +3640,10 @@
       <c r="L21" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="M21" s="29" t="s">
+      <c r="M21" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N21" s="30"/>
+      <c r="N21" s="35"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="5" t="s">
@@ -3483,10 +3680,10 @@
       <c r="L22" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="M22" s="29" t="s">
+      <c r="M22" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N22" s="30"/>
+      <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="5" t="s">
@@ -3523,10 +3720,10 @@
       <c r="L23" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="M23" s="29" t="s">
+      <c r="M23" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N23" s="30"/>
+      <c r="N23" s="35"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="5" t="s">
@@ -3563,10 +3760,10 @@
       <c r="L24" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="M24" s="29" t="s">
+      <c r="M24" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N24" s="30"/>
+      <c r="N24" s="35"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="5" t="s">
@@ -3603,10 +3800,10 @@
       <c r="L25" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="M25" s="29" t="s">
+      <c r="M25" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="N25" s="30"/>
+      <c r="N25" s="35"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A26" s="5" t="s">
@@ -3643,10 +3840,10 @@
       <c r="L26" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="M26" s="29" t="s">
+      <c r="M26" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="N26" s="30"/>
+      <c r="N26" s="35"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="5" t="s">
@@ -3683,10 +3880,10 @@
       <c r="L27" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="M27" s="29" t="s">
+      <c r="M27" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="N27" s="30"/>
+      <c r="N27" s="35"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="5" t="s">
@@ -3723,10 +3920,10 @@
       <c r="L28" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="M28" s="29" t="s">
+      <c r="M28" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="N28" s="30"/>
+      <c r="N28" s="35"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="5" t="s">
@@ -3763,10 +3960,10 @@
       <c r="L29" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="M29" s="29" t="s">
+      <c r="M29" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="N29" s="30"/>
+      <c r="N29" s="35"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="5" t="s">
@@ -3803,10 +4000,10 @@
       <c r="L30" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="M30" s="29" t="s">
+      <c r="M30" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="N30" s="30"/>
+      <c r="N30" s="35"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="5" t="s">
@@ -3843,10 +4040,10 @@
       <c r="L31" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="M31" s="29" t="s">
+      <c r="M31" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="N31" s="30"/>
+      <c r="N31" s="35"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="5" t="s">
@@ -7617,10 +7814,10 @@
       <c r="B133" s="28" t="s">
         <v>645</v>
       </c>
-      <c r="C133" s="31" t="s">
+      <c r="C133" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D133" s="32" t="s">
+      <c r="D133" s="31" t="s">
         <v>17</v>
       </c>
       <c r="J133" s="26" t="s">
@@ -7649,7 +7846,7 @@
       <c r="D134" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F134" s="33" t="s">
+      <c r="F134" s="32" t="s">
         <v>651</v>
       </c>
       <c r="G134" s="2" t="s">
@@ -7658,7 +7855,7 @@
       <c r="H134" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="J134" s="32" t="s">
+      <c r="J134" s="31" t="s">
         <v>653</v>
       </c>
       <c r="K134" s="28" t="s">
@@ -7678,10 +7875,10 @@
       <c r="B135" s="28" t="s">
         <v>656</v>
       </c>
-      <c r="C135" s="31" t="s">
+      <c r="C135" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="D135" s="32" t="s">
+      <c r="D135" s="31" t="s">
         <v>156</v>
       </c>
       <c r="E135" s="10" t="s">
@@ -7696,7 +7893,7 @@
       <c r="H135" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J135" s="32" t="s">
+      <c r="J135" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K135" s="28" t="s">
@@ -7716,19 +7913,19 @@
       <c r="C136" s="28" t="s">
         <v>661</v>
       </c>
-      <c r="D136" s="32" t="s">
+      <c r="D136" s="31" t="s">
         <v>662</v>
       </c>
       <c r="E136" s="28" t="s">
         <v>663</v>
       </c>
-      <c r="F136" s="33" t="s">
+      <c r="F136" s="32" t="s">
         <v>664</v>
       </c>
-      <c r="G136" s="34" t="s">
+      <c r="G136" s="33" t="s">
         <v>665</v>
       </c>
-      <c r="J136" s="32" t="s">
+      <c r="J136" s="31" t="s">
         <v>36</v>
       </c>
       <c r="K136" s="28" t="s">
@@ -7748,25 +7945,25 @@
       <c r="B137" s="28" t="s">
         <v>669</v>
       </c>
-      <c r="C137" s="31" t="s">
+      <c r="C137" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="D137" s="32" t="s">
+      <c r="D137" s="31" t="s">
         <v>229</v>
       </c>
       <c r="E137" s="28" t="s">
         <v>670</v>
       </c>
-      <c r="F137" s="33" t="s">
+      <c r="F137" s="32" t="s">
         <v>671</v>
       </c>
-      <c r="G137" s="34" t="s">
+      <c r="G137" s="33" t="s">
         <v>672</v>
       </c>
-      <c r="H137" s="34" t="s">
+      <c r="H137" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I137" s="34" t="s">
+      <c r="I137" s="33" t="s">
         <v>673</v>
       </c>
       <c r="K137" s="28" t="s">
@@ -7795,16 +7992,16 @@
       <c r="E138" s="28" t="s">
         <v>678</v>
       </c>
-      <c r="F138" s="33" t="s">
+      <c r="F138" s="32" t="s">
         <v>651</v>
       </c>
-      <c r="G138" s="34" t="s">
+      <c r="G138" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="H138" s="34" t="s">
+      <c r="H138" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="J138" s="32" t="s">
+      <c r="J138" s="31" t="s">
         <v>300</v>
       </c>
       <c r="K138" s="28" t="s">
@@ -7824,25 +8021,25 @@
       <c r="B139" s="28" t="s">
         <v>682</v>
       </c>
-      <c r="C139" s="31" t="s">
+      <c r="C139" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D139" s="32" t="s">
+      <c r="D139" s="31" t="s">
         <v>17</v>
       </c>
       <c r="E139" s="28" t="s">
         <v>683</v>
       </c>
-      <c r="F139" s="33" t="s">
+      <c r="F139" s="32" t="s">
         <v>684</v>
       </c>
-      <c r="G139" s="34" t="s">
+      <c r="G139" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="H139" s="34" t="s">
+      <c r="H139" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="J139" s="32" t="s">
+      <c r="J139" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K139" s="28" t="s">
@@ -7859,10 +8056,10 @@
       <c r="B140" s="28" t="s">
         <v>688</v>
       </c>
-      <c r="C140" s="31" t="s">
+      <c r="C140" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D140" s="32" t="s">
+      <c r="D140" s="31" t="s">
         <v>196</v>
       </c>
       <c r="E140" s="16" t="s">
@@ -7878,7 +8075,7 @@
         <v>170</v>
       </c>
       <c r="I140" s="14"/>
-      <c r="J140" s="32" t="s">
+      <c r="J140" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K140" s="28" t="s">
@@ -7895,25 +8092,25 @@
       <c r="B141" s="28" t="s">
         <v>692</v>
       </c>
-      <c r="C141" s="31" t="s">
+      <c r="C141" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D141" s="32" t="s">
+      <c r="D141" s="31" t="s">
         <v>196</v>
       </c>
       <c r="E141" s="28" t="s">
         <v>693</v>
       </c>
-      <c r="F141" s="33" t="s">
+      <c r="F141" s="32" t="s">
         <v>694</v>
       </c>
-      <c r="G141" s="32" t="s">
+      <c r="G141" s="31" t="s">
         <v>695</v>
       </c>
-      <c r="H141" s="32" t="s">
+      <c r="H141" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="J141" s="32" t="s">
+      <c r="J141" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K141" s="28" t="s">
@@ -7930,25 +8127,25 @@
       <c r="B142" s="28" t="s">
         <v>698</v>
       </c>
-      <c r="C142" s="31" t="s">
+      <c r="C142" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D142" s="32" t="s">
+      <c r="D142" s="31" t="s">
         <v>196</v>
       </c>
       <c r="E142" s="28" t="s">
         <v>699</v>
       </c>
-      <c r="F142" s="33" t="s">
+      <c r="F142" s="32" t="s">
         <v>700</v>
       </c>
-      <c r="G142" s="32" t="s">
+      <c r="G142" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="H142" s="32" t="s">
+      <c r="H142" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="J142" s="32" t="s">
+      <c r="J142" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K142" s="28" t="s">
@@ -7974,16 +8171,16 @@
       <c r="E143" s="28" t="s">
         <v>699</v>
       </c>
-      <c r="F143" s="33" t="s">
+      <c r="F143" s="32" t="s">
         <v>700</v>
       </c>
-      <c r="G143" s="32" t="s">
+      <c r="G143" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="H143" s="32" t="s">
+      <c r="H143" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="J143" s="32" t="s">
+      <c r="J143" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K143" s="28" t="s">
@@ -8000,25 +8197,25 @@
       <c r="B144" s="28" t="s">
         <v>703</v>
       </c>
-      <c r="C144" s="31" t="s">
+      <c r="C144" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D144" s="32" t="s">
+      <c r="D144" s="31" t="s">
         <v>196</v>
       </c>
       <c r="E144" s="28" t="s">
         <v>704</v>
       </c>
-      <c r="F144" s="33" t="s">
+      <c r="F144" s="32" t="s">
         <v>705</v>
       </c>
-      <c r="G144" s="32" t="s">
+      <c r="G144" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="H144" s="32" t="s">
+      <c r="H144" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="J144" s="32" t="s">
+      <c r="J144" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K144" s="24" t="s">
@@ -8031,29 +8228,29 @@
         <v>691</v>
       </c>
     </row>
-    <row r="145" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="145" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B145" s="28" t="s">
         <v>708</v>
       </c>
-      <c r="C145" s="31" t="s">
+      <c r="C145" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D145" s="32" t="s">
+      <c r="D145" s="31" t="s">
         <v>196</v>
       </c>
       <c r="E145" s="28" t="s">
         <v>709</v>
       </c>
-      <c r="F145" s="33" t="s">
+      <c r="F145" s="32" t="s">
         <v>710</v>
       </c>
-      <c r="G145" s="32" t="s">
+      <c r="G145" s="31" t="s">
         <v>711</v>
       </c>
-      <c r="H145" s="32" t="s">
+      <c r="H145" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="J145" s="32" t="s">
+      <c r="J145" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K145" s="28" t="s">
@@ -8066,29 +8263,29 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="146" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B146" s="28" t="s">
         <v>714</v>
       </c>
-      <c r="C146" s="31" t="s">
+      <c r="C146" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="D146" s="32" t="s">
+      <c r="D146" s="31" t="s">
         <v>196</v>
       </c>
       <c r="E146" s="28" t="s">
         <v>715</v>
       </c>
-      <c r="F146" s="33" t="s">
+      <c r="F146" s="32" t="s">
         <v>716</v>
       </c>
-      <c r="G146" s="32" t="s">
+      <c r="G146" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="H146" s="32" t="s">
+      <c r="H146" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="J146" s="32" t="s">
+      <c r="J146" s="31" t="s">
         <v>22</v>
       </c>
       <c r="K146" s="28" t="s">
@@ -8101,54 +8298,479 @@
         <v>691</v>
       </c>
     </row>
-    <row r="147" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B147" s="28" t="s">
+    <row r="147" spans="2:14" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B147" s="36" t="s">
         <v>719</v>
       </c>
-      <c r="C147" s="31" t="s">
+      <c r="C147" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="D147" s="32" t="s">
+      <c r="D147" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="E147" s="28" t="s">
+      <c r="E147" s="36" t="s">
         <v>720</v>
       </c>
-      <c r="F147" s="33" t="s">
+      <c r="F147" s="39" t="s">
         <v>721</v>
       </c>
-      <c r="G147" s="32" t="s">
+      <c r="G147" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="H147" s="32" t="s">
+      <c r="H147" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="J147" s="32" t="s">
+      <c r="J147" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="K147" s="28" t="s">
+      <c r="K147" s="36" t="s">
         <v>722</v>
       </c>
-      <c r="L147" s="28" t="s">
+      <c r="L147" s="36" t="s">
         <v>723</v>
       </c>
-      <c r="M147" s="28" t="s">
+      <c r="M147" s="36" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="148" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="149" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="150" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="151" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="152" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="153" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="154" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="155" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="156" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="157" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="158" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="159" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
-    <row r="160" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+    <row r="148" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B148" s="29" t="s">
+        <v>724</v>
+      </c>
+      <c r="C148" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D148" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E148" s="29" t="s">
+        <v>725</v>
+      </c>
+      <c r="F148" s="32" t="s">
+        <v>726</v>
+      </c>
+      <c r="G148" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H148" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J148" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K148" s="29" t="s">
+        <v>727</v>
+      </c>
+      <c r="L148" s="29" t="s">
+        <v>728</v>
+      </c>
+      <c r="M148" s="29" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="149" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B149" s="29" t="s">
+        <v>730</v>
+      </c>
+      <c r="C149" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D149" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E149" s="29" t="s">
+        <v>725</v>
+      </c>
+      <c r="F149" s="32" t="s">
+        <v>726</v>
+      </c>
+      <c r="G149" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H149" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I149" s="29"/>
+      <c r="J149" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K149" s="29" t="s">
+        <v>732</v>
+      </c>
+      <c r="L149" s="29" t="s">
+        <v>731</v>
+      </c>
+      <c r="M149" s="29" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="150" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B150" s="29" t="s">
+        <v>734</v>
+      </c>
+      <c r="C150" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D150" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E150" s="29" t="s">
+        <v>725</v>
+      </c>
+      <c r="F150" s="32" t="s">
+        <v>726</v>
+      </c>
+      <c r="G150" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H150" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J150" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K150" s="29" t="s">
+        <v>735</v>
+      </c>
+      <c r="L150" s="29" t="s">
+        <v>736</v>
+      </c>
+      <c r="M150" s="29" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="151" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B151" s="29" t="s">
+        <v>738</v>
+      </c>
+      <c r="C151" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D151" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E151" s="29" t="s">
+        <v>739</v>
+      </c>
+      <c r="F151" s="32" t="s">
+        <v>740</v>
+      </c>
+      <c r="G151" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H151" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J151" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K151" s="29" t="s">
+        <v>741</v>
+      </c>
+      <c r="L151" s="29" t="s">
+        <v>742</v>
+      </c>
+      <c r="M151" s="29" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="152" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B152" s="29" t="s">
+        <v>744</v>
+      </c>
+      <c r="C152" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D152" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E152" s="29" t="s">
+        <v>745</v>
+      </c>
+      <c r="F152" s="32" t="s">
+        <v>747</v>
+      </c>
+      <c r="G152" s="29" t="s">
+        <v>746</v>
+      </c>
+      <c r="H152" s="29" t="s">
+        <v>748</v>
+      </c>
+      <c r="J152" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K152" s="29" t="s">
+        <v>749</v>
+      </c>
+      <c r="L152" s="29" t="s">
+        <v>750</v>
+      </c>
+      <c r="M152" s="29" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="153" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B153" s="29" t="s">
+        <v>752</v>
+      </c>
+      <c r="C153" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D153" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E153" s="29" t="s">
+        <v>745</v>
+      </c>
+      <c r="F153" s="32" t="s">
+        <v>747</v>
+      </c>
+      <c r="G153" s="29" t="s">
+        <v>746</v>
+      </c>
+      <c r="H153" s="29" t="s">
+        <v>748</v>
+      </c>
+      <c r="J153" s="31" t="s">
+        <v>754</v>
+      </c>
+      <c r="K153" s="29" t="s">
+        <v>753</v>
+      </c>
+      <c r="L153" s="29" t="s">
+        <v>755</v>
+      </c>
+      <c r="M153" s="29" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="154" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B154" s="29" t="s">
+        <v>756</v>
+      </c>
+      <c r="C154" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D154" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E154" s="29" t="s">
+        <v>573</v>
+      </c>
+      <c r="F154" s="32" t="s">
+        <v>747</v>
+      </c>
+      <c r="G154" s="29" t="s">
+        <v>757</v>
+      </c>
+      <c r="H154" s="29" t="s">
+        <v>758</v>
+      </c>
+      <c r="J154" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K154" s="29" t="s">
+        <v>759</v>
+      </c>
+      <c r="L154" s="29" t="s">
+        <v>760</v>
+      </c>
+      <c r="M154" s="29" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="155" spans="2:14" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B155" s="29" t="s">
+        <v>756</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E155" s="29" t="s">
+        <v>573</v>
+      </c>
+      <c r="F155" s="32" t="s">
+        <v>747</v>
+      </c>
+      <c r="G155" s="29" t="s">
+        <v>757</v>
+      </c>
+      <c r="H155" s="29" t="s">
+        <v>758</v>
+      </c>
+      <c r="J155" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K155" s="29" t="s">
+        <v>759</v>
+      </c>
+      <c r="L155" s="29" t="s">
+        <v>760</v>
+      </c>
+      <c r="M155" s="29" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="156" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B156" s="29" t="s">
+        <v>762</v>
+      </c>
+      <c r="C156" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D156" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E156" s="29" t="s">
+        <v>763</v>
+      </c>
+      <c r="F156" s="32" t="s">
+        <v>764</v>
+      </c>
+      <c r="G156" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="H156" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="J156" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K156" s="29" t="s">
+        <v>766</v>
+      </c>
+      <c r="L156" s="29" t="s">
+        <v>767</v>
+      </c>
+      <c r="M156" s="29" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="157" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B157" s="29" t="s">
+        <v>769</v>
+      </c>
+      <c r="C157" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D157" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E157" s="29" t="s">
+        <v>763</v>
+      </c>
+      <c r="F157" s="32" t="s">
+        <v>764</v>
+      </c>
+      <c r="G157" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="H157" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="J157" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K157" s="29" t="s">
+        <v>770</v>
+      </c>
+      <c r="L157" s="29" t="s">
+        <v>771</v>
+      </c>
+      <c r="M157" s="29" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="158" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B158" s="29" t="s">
+        <v>773</v>
+      </c>
+      <c r="C158" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D158" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J158" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K158" s="29" t="s">
+        <v>774</v>
+      </c>
+      <c r="L158" s="29" t="s">
+        <v>775</v>
+      </c>
+      <c r="M158" s="29" t="s">
+        <v>776</v>
+      </c>
+      <c r="N158" s="29" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="159" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B159" s="29" t="s">
+        <v>777</v>
+      </c>
+      <c r="C159" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D159" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J159" s="31" t="s">
+        <v>393</v>
+      </c>
+      <c r="K159" s="29" t="s">
+        <v>778</v>
+      </c>
+      <c r="L159" s="29" t="s">
+        <v>779</v>
+      </c>
+      <c r="M159" s="29" t="s">
+        <v>780</v>
+      </c>
+      <c r="N159" s="29" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="160" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B160" s="29" t="s">
+        <v>781</v>
+      </c>
+      <c r="C160" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D160" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E160" t="s">
+        <v>782</v>
+      </c>
+      <c r="F160" s="32" t="s">
+        <v>740</v>
+      </c>
+      <c r="G160" t="s">
+        <v>20</v>
+      </c>
+      <c r="H160" t="s">
+        <v>21</v>
+      </c>
+      <c r="J160" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K160" s="29" t="s">
+        <v>783</v>
+      </c>
+      <c r="L160" s="29" t="s">
+        <v>784</v>
+      </c>
+      <c r="M160" s="29" t="s">
+        <v>785</v>
+      </c>
+    </row>
     <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
     <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -8990,26 +9612,6 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="M31:N31"/>
@@ -9020,6 +9622,26 @@
     <mergeCell ref="M27:N27"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>

</xml_diff>